<commit_message>
update eve benchmark report
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/201912/jsliu__bank_test_&_city_(HF)(201912)_EVE.xlsx
+++ b/lib/report/benchmark_report/web14/exl/201912/jsliu__bank_test_&_city_(HF)(201912)_EVE.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t xml:space="preserve">Economic Value of Equity (EVE) Report </t>
   </si>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Cycle: December, 2019        Evaluation Date: December 31, 2019</t>
   </si>
   <si>
-    <t>Print on: 03/18/20 3:30:55 PM</t>
+    <t>Print on: 03/24/20 12:38:52 PM</t>
   </si>
   <si>
     <t>Comments:</t>
@@ -133,6 +133,181 @@
   </si>
   <si>
     <t>The % change in value per 100 basis point shifts in the yield curve, measuring value sensitivity</t>
+  </si>
+  <si>
+    <t>Capital Assets</t>
+  </si>
+  <si>
+    <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Glossary:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.    CUSIP: CUSIP customized for and assigned to the appropriate security;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.    Down N BP: Present value if the yield curve shocks down N BP;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.    Base Case (0 BP): Present value as current yield curve;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.    Up N BP: Present value if the yield curve shocks up N BP;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.    BC/FV (%) = (Base Case - Accrued Interest) / Face Value * 100%;</t>
+  </si>
+  <si>
+    <t>[Note: The inconsequence principal (such as principal of Fixed-Rate Servicing, Adjustable-Rate Servicing) are treated as zero when plusing.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.    Duration(Dur) = (PV if yield curve shocks down 0.1% - PV if yield curve shocks up 0.1%) / (2 * PV * 0.1%), PV means present value;</t>
+  </si>
+  <si>
+    <t>DV01 for OBS items (the values with *): DV01 = (PV if yield curve shocks down 0.1% - PV if yield curve shocks up 0.1%) / (2 * 10000 * 0.1%), PV means present value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.    Convexity(Conv) = (PV if yield curve shocks up 0.1% + PV if yield curve shocks down 0.1% - 2 * PV) / (PV * 0.1% * 0.1%) / 100, PV means present value.</t>
+  </si>
+  <si>
+    <t>Base Case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flattener is an interest rate scenario where the shock of the yield curve is "non-parallel". A 300 basis point shock of a yield curve assumes that the yield curve makes an instantaneous upward shift of 300 basis points, as defined by the Table 1 below. In this case, the yield curve has made a parallel shift.
+By way of contrast, a flattener requires the yield curve to shift not by a constant value, such as 300 basis points, along the entire yield curve. Instead a flattener requires the short term rate shifts more than the long term rate. In particular, the scenario requires the overnight rate to shift upward 300 basis points and the 10 year rate to shift upward with a smaller amount of 100 basis points. The rates shift less as the term increases along the yield curve, with 20 basis points less for every year. Table 1 presents the precise rate shift for each term.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1. The shifts of 300 basis point parallel shock and the flattener non-parallel shock in basis points </t>
+  </si>
+  <si>
+    <t>Term in years</t>
+  </si>
+  <si>
+    <t>Overnight rate</t>
+  </si>
+  <si>
+    <t>1yr</t>
+  </si>
+  <si>
+    <t>2yr</t>
+  </si>
+  <si>
+    <t>3yr</t>
+  </si>
+  <si>
+    <t>4yr</t>
+  </si>
+  <si>
+    <t>5yr</t>
+  </si>
+  <si>
+    <t>6yr</t>
+  </si>
+  <si>
+    <t>7yr</t>
+  </si>
+  <si>
+    <t>8yr</t>
+  </si>
+  <si>
+    <t>9yr</t>
+  </si>
+  <si>
+    <t>10yr</t>
+  </si>
+  <si>
+    <t>10yr+</t>
+  </si>
+  <si>
+    <t>300bpt shock</t>
+  </si>
+  <si>
+    <t>The resulting yield curve after a flattener shift is depicted in Figure 1 as of Dec 31,2019. The blue line is the prevailing yield curve. The red line is the simulated yield curve scenario of the flattener. As Figure 1 shows, the resulting yield curve is relatively flat where the rates are approximately 3% for all the terms up to 10 year. Hence, this scenario is called a flattener.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 1.  Prevailing Yield Curve as of Dec,2019 and the Yield Curve of the Flattener Scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flattener </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The flattener scenario is important to interest rate risk analysis for two reasons. (1) Historically, when the yield curve begins to rise, the short term rates tend to move up faster than the long term rate. Therefore, the flattener is a probable scenario. (2) Many community banks have short term funding of long term fixed rate mortgage loans.  When the yield curve flattens as depicted in Figure 1, then the net interest margin would be tightened. Furthermore, the fixed rate mortgage loans on the book would have a rate lower than the market rate, resulting in the mortgagors holding on to the relatively low borrowing cost for a longer period. This is an adverse scenario that community bank should be aware of.</t>
+  </si>
+  <si>
+    <t>For the reasons given above, banks should monitor the impact of the flattener on the percentage change of Economic Value of Equity (EVE) and percentage change of Net Interest Income (NII) over 12 months and 24 months. The impact should not be much more adverse than that of the scenario of the 200 basis point parallel shock. The percentage of EVE measures the EVE duration risk and the option risk embedded on the balance sheet. Percentage change of NII measures the repricing risk of the balance sheet.</t>
+  </si>
+  <si>
+    <t>Calculation Setting:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valuation Paths: 1          Simulation Paths: 1          Valuation Method: LPS          OAS Type: TSY          Price Model: HoLeeG1F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yield Curve: Treasury          Vol Curve: SwaptionHoLeeG1Factor          Parameter Set: Default          CPR Shocks (BP): 0          CDR Shocks (BP): 0</t>
+  </si>
+  <si>
+    <t>Maturity* (with the suffix *) indicates that some items are not taken in averaging the weighted average maturity.</t>
+  </si>
+  <si>
+    <t>The followings show the details about the amount that are not taken into account for the weighted average maturity in the chart of accounts.</t>
+  </si>
+  <si>
+    <t>Total assets(Amounts in 000s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Premises and fixed assets (including capitalized leases) : 1,618.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other real estate owned : 81.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Others : 1,209.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      LESS: Allowance for loan and lease losses : -725.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Other assets : 2,183.00</t>
+  </si>
+  <si>
+    <t>Total assets : 2,183.00</t>
+  </si>
+  <si>
+    <t>Total liabilities(Amounts in 000s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      MMDAs : 1,603.51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Passbook Accounts : 24,018.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Transaction Accounts : 8,628.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Noninterest-bearing Accounts : 14,945.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Deposits : 49,196.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Others : 371.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Other liabilities : 371.00</t>
+  </si>
+  <si>
+    <t>Total liabilities : 49,567.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jsliu  bank test &amp; city (HF)-201912 : -47,384.72</t>
+  </si>
+  <si>
+    <t>Print on: 03/24/20 12:38:53 PM</t>
   </si>
   <si>
     <t>Sector</t>
@@ -314,175 +489,6 @@
   </si>
   <si>
     <t xml:space="preserve">jsliu  bank test &amp; city (HF)-201912</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Glossary:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.    CUSIP: CUSIP customized for and assigned to the appropriate security;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.    Down N BP: Present value if the yield curve shocks down N BP;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.    Base Case (0 BP): Present value as current yield curve;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.    Up N BP: Present value if the yield curve shocks up N BP;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.    BC/FV (%) = (Base Case - Accrued Interest) / Face Value * 100%;</t>
-  </si>
-  <si>
-    <t>[Note: The inconsequence principal (such as principal of Fixed-Rate Servicing, Adjustable-Rate Servicing) are treated as zero when plusing.]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.    Duration(Dur) = (PV if yield curve shocks down 0.1% - PV if yield curve shocks up 0.1%) / (2 * PV * 0.1%), PV means present value;</t>
-  </si>
-  <si>
-    <t>DV01 for OBS items (the values with *): DV01 = (PV if yield curve shocks down 0.1% - PV if yield curve shocks up 0.1%) / (2 * 10000 * 0.1%), PV means present value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.    Convexity(Conv) = (PV if yield curve shocks up 0.1% + PV if yield curve shocks down 0.1% - 2 * PV) / (PV * 0.1% * 0.1%) / 100, PV means present value.</t>
-  </si>
-  <si>
-    <t>Base Case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flattener is an interest rate scenario where the shock of the yield curve is "non-parallel". A 300 basis point shock of a yield curve assumes that the yield curve makes an instantaneous upward shift of 300 basis points, as defined by the Table 1 below. In this case, the yield curve has made a parallel shift.
-By way of contrast, a flattener requires the yield curve to shift not by a constant value, such as 300 basis points, along the entire yield curve. Instead a flattener requires the short term rate shifts more than the long term rate. In particular, the scenario requires the overnight rate to shift upward 300 basis points and the 10 year rate to shift upward with a smaller amount of 100 basis points. The rates shift less as the term increases along the yield curve, with 20 basis points less for every year. Table 1 presents the precise rate shift for each term.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 1. The shifts of 300 basis point parallel shock and the flattener non-parallel shock in basis points </t>
-  </si>
-  <si>
-    <t>Term in years</t>
-  </si>
-  <si>
-    <t>Overnight rate</t>
-  </si>
-  <si>
-    <t>1yr</t>
-  </si>
-  <si>
-    <t>2yr</t>
-  </si>
-  <si>
-    <t>3yr</t>
-  </si>
-  <si>
-    <t>4yr</t>
-  </si>
-  <si>
-    <t>5yr</t>
-  </si>
-  <si>
-    <t>6yr</t>
-  </si>
-  <si>
-    <t>7yr</t>
-  </si>
-  <si>
-    <t>8yr</t>
-  </si>
-  <si>
-    <t>9yr</t>
-  </si>
-  <si>
-    <t>10yr</t>
-  </si>
-  <si>
-    <t>10yr+</t>
-  </si>
-  <si>
-    <t>300bpt shock</t>
-  </si>
-  <si>
-    <t>The resulting yield curve after a flattener shift is depicted in Figure 1 as of Dec 31,2019. The blue line is the prevailing yield curve. The red line is the simulated yield curve scenario of the flattener. As Figure 1 shows, the resulting yield curve is relatively flat where the rates are approximately 3% for all the terms up to 10 year. Hence, this scenario is called a flattener.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Figure 1.  Prevailing Yield Curve as of Dec,2019 and the Yield Curve of the Flattener Scenario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flattener </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The flattener scenario is important to interest rate risk analysis for two reasons. (1) Historically, when the yield curve begins to rise, the short term rates tend to move up faster than the long term rate. Therefore, the flattener is a probable scenario. (2) Many community banks have short term funding of long term fixed rate mortgage loans.  When the yield curve flattens as depicted in Figure 1, then the net interest margin would be tightened. Furthermore, the fixed rate mortgage loans on the book would have a rate lower than the market rate, resulting in the mortgagors holding on to the relatively low borrowing cost for a longer period. This is an adverse scenario that community bank should be aware of.</t>
-  </si>
-  <si>
-    <t>For the reasons given above, banks should monitor the impact of the flattener on the percentage change of Economic Value of Equity (EVE) and percentage change of Net Interest Income (NII) over 12 months and 24 months. The impact should not be much more adverse than that of the scenario of the 200 basis point parallel shock. The percentage of EVE measures the EVE duration risk and the option risk embedded on the balance sheet. Percentage change of NII measures the repricing risk of the balance sheet.</t>
-  </si>
-  <si>
-    <t>Calculation Setting:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valuation Paths: 1          Simulation Paths: 1          Valuation Method: LPS          OAS Type: TSY          Price Model: HoLeeG1F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yield Curve: Treasury          Vol Curve: SwaptionHoLeeG1Factor          Parameter Set: Default          CPR Shocks (BP): 0          CDR Shocks (BP): 0</t>
-  </si>
-  <si>
-    <t>Maturity* (with the suffix *) indicates that some items are not taken in averaging the weighted average maturity.</t>
-  </si>
-  <si>
-    <t>The followings show the details about the amount that are not taken into account for the weighted average maturity in the chart of accounts.</t>
-  </si>
-  <si>
-    <t>Total assets(Amounts in 000s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Premises and fixed assets (including capitalized leases) : 1,618.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Other real estate owned : 81.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Others : 1,209.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      LESS: Allowance for loan and lease losses : -725.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Other assets : 2,183.00</t>
-  </si>
-  <si>
-    <t>Total assets : 2,183.00</t>
-  </si>
-  <si>
-    <t>Total liabilities(Amounts in 000s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      MMDAs : 1,603.51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Passbook Accounts : 24,018.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Transaction Accounts : 8,628.82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Noninterest-bearing Accounts : 14,945.56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Deposits : 49,196.72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Others : 371.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Other liabilities : 371.00</t>
-  </si>
-  <si>
-    <t>Total liabilities : 49,567.72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jsliu  bank test &amp; city (HF)-201912 : -47,384.72</t>
-  </si>
-  <si>
-    <t>Disclaimer</t>
   </si>
 </sst>
 </file>
@@ -2672,8 +2678,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.36585825155227925"/>
-          <c:y val="3.2453325409796188E-2"/>
+          <c:x val="0.36585825155227936"/>
+          <c:y val="3.2453325409796202E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2775,8 +2781,8 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="103373056"/>
-        <c:axId val="103374848"/>
+        <c:axId val="92031232"/>
+        <c:axId val="92037120"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2943,7 +2949,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103373056"/>
+        <c:axId val="92031232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2981,14 +2987,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103374848"/>
+        <c:crossAx val="92037120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103374848"/>
+        <c:axId val="92037120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3034,7 +3040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103373056"/>
+        <c:crossAx val="92031232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3078,7 +3084,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000766" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000766" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000777" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000777" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3139,8 +3145,8 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="101934208"/>
-        <c:axId val="101935744"/>
+        <c:axId val="92048384"/>
+        <c:axId val="92074752"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3157,7 +3163,7 @@
           </c:spPr>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary'!E9</c:f>
+              <c:f>'Summary'!H28</c:f>
               <c:strCache>
                 <c:ptCount val="0"/>
               </c:strCache>
@@ -3185,17 +3191,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary'!$E$10:$E$19</c:f>
+              <c:f>'Summary'!$H$29:$H$38</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </ser>
         <c:smooth val="0"/>
-        <c:axId val="101935745"/>
-        <c:axId val="101935746"/>
+        <c:axId val="92074753"/>
+        <c:axId val="92074754"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101934208"/>
+        <c:axId val="92048384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3233,14 +3239,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101935744"/>
+        <c:crossAx val="92074752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101935744"/>
+        <c:axId val="92074752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="12"/>
@@ -3306,26 +3312,26 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101934208"/>
+        <c:crossAx val="92048384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="101935745"/>
+        <c:axId val="92074753"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="101935746"/>
+        <c:crossAx val="92074754"/>
         <c:crosses val="autoZero"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101935746"/>
+        <c:axId val="92074754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="12000"/>
+          <c:min val="89000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -3340,7 +3346,7 @@
                     <a:latin typeface="Ubuntu"/>
                     <a:cs typeface="Ubuntu"/>
                   </a:rPr>
-                  <a:t>$Amount</a:t>
+                  <a:t>Capital Assets</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3354,7 +3360,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="101935745"/>
+        <c:crossAx val="92074753"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3433,7 +3439,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000788" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000788" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000799" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000799" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3478,6 +3484,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3581,11 +3588,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </ser>
-        <c:axId val="108139648"/>
-        <c:axId val="108141184"/>
+        <c:axId val="93168000"/>
+        <c:axId val="93169536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108139648"/>
+        <c:axId val="93168000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3623,12 +3630,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108141184"/>
+        <c:crossAx val="93169536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108141184"/>
+        <c:axId val="93169536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3668,7 +3675,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="6.6519673399882172E-3"/>
-              <c:y val="0.37395733983956386"/>
+              <c:y val="0.37395733983956392"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -3696,7 +3703,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108139648"/>
+        <c:crossAx val="93168000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3710,6 +3717,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -3743,7 +3751,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000788" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000788" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000799" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000799" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3950,11 +3958,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="108182912"/>
-        <c:axId val="108197376"/>
+        <c:axId val="93276800"/>
+        <c:axId val="93287168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108182912"/>
+        <c:axId val="93276800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3995,12 +4003,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108197376"/>
+        <c:crossAx val="93287168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108197376"/>
+        <c:axId val="93287168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4021,7 +4029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108182912"/>
+        <c:crossAx val="93276800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4058,20 +4066,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>843915</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63FBC450-9F79-4EF8-B62B-A123B7A640F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63FBC450-9F79-4EF8-B62B-A123B7A640F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4092,22 +4100,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
+      <xdr:colOff>981075</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>426175</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>473800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64304E9D-A8BA-4370-84B4-25B00CBFDDDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{64304E9D-A8BA-4370-84B4-25B00CBFDDDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4148,7 +4156,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63FBC450-9F79-4EF8-B62B-A123B7A640F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63FBC450-9F79-4EF8-B62B-A123B7A640F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4219,7 +4227,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{285B5163-0187-4EEC-980D-9FB4FB5791D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{285B5163-0187-4EEC-980D-9FB4FB5791D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4689,7 +4697,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection sqref="A1:M1"/>
@@ -5129,6 +5137,66 @@
       <c r="F26" s="254"/>
       <c r="G26" s="251"/>
     </row>
+    <row r="28" ht="9.95" customHeight="1">
+      <c r="H28" s="227" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" ht="9.95" customHeight="1">
+      <c r="H29" s="249">
+        <v>116338.42734398923</v>
+      </c>
+    </row>
+    <row r="30" ht="9.95" customHeight="1">
+      <c r="H30" s="249">
+        <v>114795.2348916972</v>
+      </c>
+    </row>
+    <row r="31" ht="9.95" customHeight="1">
+      <c r="H31" s="249">
+        <v>113509.08046013973</v>
+      </c>
+    </row>
+    <row r="32" ht="9.95" customHeight="1">
+      <c r="H32" s="249">
+        <v>112153.55805661147</v>
+      </c>
+    </row>
+    <row r="33" ht="9.95" customHeight="1">
+      <c r="H33" s="249">
+        <v>110781.24529712075</v>
+      </c>
+    </row>
+    <row r="34" ht="9.95" customHeight="1">
+      <c r="H34" s="249">
+        <v>109494.96036181765</v>
+      </c>
+    </row>
+    <row r="35" ht="9.95" customHeight="1">
+      <c r="H35" s="249">
+        <v>107045.55042771756</v>
+      </c>
+    </row>
+    <row r="36" ht="9.95" customHeight="1">
+      <c r="H36" s="249">
+        <v>103448.56351612024</v>
+      </c>
+    </row>
+    <row r="37" ht="9.95" customHeight="1">
+      <c r="H37" s="249">
+        <v>99546.1010337897</v>
+      </c>
+    </row>
+    <row r="38" ht="9.95" customHeight="1">
+      <c r="H38" s="249">
+        <v>106388.637195554</v>
+      </c>
+    </row>
+    <row r="39" ht="9.95" customHeight="1">
+      <c r="H39" s="249">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A21:M21"/>
@@ -5146,8 +5214,8 @@
     <oddFooter>&amp;C&amp;"Ubuntu,Regular"&amp;8&amp;K00-048Thomas Ho Company Ltd.
 https://www.thcdecisions.com | lxu@thc.net.cn&amp;R&amp;"Ubuntu,Regular"&amp;8&amp;K00-048&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawingHF r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawingHF r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -5232,19 +5300,19 @@
       <c r="K3" s="237"/>
       <c r="L3" s="237"/>
       <c r="R3" s="239" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" ht="8.1" customHeight="1"/>
     <row r="5" ht="28.5">
       <c r="A5" s="233" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="B5" s="236" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="C5" s="236" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="D5" s="238" t="s">
         <v>15</v>
@@ -5277,24 +5345,24 @@
         <v>24</v>
       </c>
       <c r="N5" s="238" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="O5" s="238" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="P5" s="236" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="236" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="R5" s="236" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="269" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="B6" s="270"/>
       <c r="C6" s="270"/>
@@ -5316,7 +5384,7 @@
     </row>
     <row r="7">
       <c r="A7" s="274" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="B7" s="275">
         <v>5.170114552357802</v>
@@ -5372,7 +5440,7 @@
     </row>
     <row r="8">
       <c r="A8" s="274" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="B8" s="275">
         <v>5.170114552357802</v>
@@ -5428,7 +5496,7 @@
     </row>
     <row r="9">
       <c r="A9" s="274" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="B9" s="275">
         <v>0.79135050639771976</v>
@@ -5484,7 +5552,7 @@
     </row>
     <row r="10">
       <c r="A10" s="279" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="B10" s="280">
         <v>37.543800160535064</v>
@@ -5540,7 +5608,7 @@
     </row>
     <row r="12">
       <c r="A12" s="269" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="B12" s="270"/>
       <c r="C12" s="270"/>
@@ -5562,7 +5630,7 @@
     </row>
     <row r="13" outlineLevel="2">
       <c r="A13" s="284" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="B13" s="242">
         <v>0</v>
@@ -5618,7 +5686,7 @@
     </row>
     <row r="14" outlineLevel="2">
       <c r="A14" s="284" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="B14" s="242">
         <v>1.55</v>
@@ -5674,7 +5742,7 @@
     </row>
     <row r="15" outlineLevel="1">
       <c r="A15" s="285" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="B15" s="286">
         <v>0.51602852009880984</v>
@@ -5730,7 +5798,7 @@
     </row>
     <row r="16" outlineLevel="2">
       <c r="A16" s="289" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="B16" s="242">
         <v>3.3044058745</v>
@@ -5786,7 +5854,7 @@
     </row>
     <row r="17" outlineLevel="2">
       <c r="A17" s="290" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="B17" s="286">
         <v>3.3044058745</v>
@@ -5842,7 +5910,7 @@
     </row>
     <row r="18" outlineLevel="2">
       <c r="A18" s="284" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="B18" s="242">
         <v>2.6785714286</v>
@@ -5898,7 +5966,7 @@
     </row>
     <row r="19" outlineLevel="2">
       <c r="A19" s="291" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="B19" s="242">
         <v>2.66782748034572</v>
@@ -5954,7 +6022,7 @@
     </row>
     <row r="20" outlineLevel="2">
       <c r="A20" s="292" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="B20" s="286">
         <v>2.66782748034572</v>
@@ -6010,7 +6078,7 @@
     </row>
     <row r="21" outlineLevel="2">
       <c r="A21" s="291" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="B21" s="242">
         <v>2.2279546278</v>
@@ -6066,7 +6134,7 @@
     </row>
     <row r="22" outlineLevel="2">
       <c r="A22" s="292" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="B22" s="286">
         <v>2.2279546278</v>
@@ -6122,7 +6190,7 @@
     </row>
     <row r="23" outlineLevel="2">
       <c r="A23" s="290" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="B23" s="286">
         <v>2.5945945946245947</v>
@@ -6178,7 +6246,7 @@
     </row>
     <row r="24" outlineLevel="1">
       <c r="A24" s="285" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="B24" s="286">
         <v>2.9723266142955755</v>
@@ -6234,7 +6302,7 @@
     </row>
     <row r="25" outlineLevel="2">
       <c r="A25" s="291" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="B25" s="242">
         <v>7.6808180531</v>
@@ -6290,7 +6358,7 @@
     </row>
     <row r="26" outlineLevel="2">
       <c r="A26" s="291" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B26" s="242">
         <v>7.6808180531</v>
@@ -6346,7 +6414,7 @@
     </row>
     <row r="27" outlineLevel="2">
       <c r="A27" s="292" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="B27" s="286">
         <v>7.6808180531</v>
@@ -6402,7 +6470,7 @@
     </row>
     <row r="28" outlineLevel="2">
       <c r="A28" s="289" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="B28" s="242">
         <v>5.0003163474</v>
@@ -6458,7 +6526,7 @@
     </row>
     <row r="29" outlineLevel="2">
       <c r="A29" s="291" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="B29" s="242">
         <v>6.6193475177</v>
@@ -6514,7 +6582,7 @@
     </row>
     <row r="30" outlineLevel="2">
       <c r="A30" s="293" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B30" s="242">
         <v>5.7629889347</v>
@@ -6570,7 +6638,7 @@
     </row>
     <row r="31" outlineLevel="2">
       <c r="A31" s="293" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B31" s="242">
         <v>6.6193475177</v>
@@ -6626,7 +6694,7 @@
     </row>
     <row r="32" outlineLevel="2">
       <c r="A32" s="294" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="B32" s="286">
         <v>5.7731989960058474</v>
@@ -6682,7 +6750,7 @@
     </row>
     <row r="33" outlineLevel="2">
       <c r="A33" s="292" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="B33" s="286">
         <v>5.8082859463737142</v>
@@ -6738,7 +6806,7 @@
     </row>
     <row r="34" outlineLevel="2">
       <c r="A34" s="291" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="B34" s="242">
         <v>5.0003163474</v>
@@ -6794,7 +6862,7 @@
     </row>
     <row r="35" outlineLevel="2">
       <c r="A35" s="291" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="B35" s="242">
         <v>5.0003163474</v>
@@ -6850,7 +6918,7 @@
     </row>
     <row r="36" outlineLevel="2">
       <c r="A36" s="292" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="B36" s="286">
         <v>5.0003163474</v>
@@ -6906,7 +6974,7 @@
     </row>
     <row r="37" outlineLevel="2">
       <c r="A37" s="290" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="B37" s="286">
         <v>5.7491116553607915</v>
@@ -6962,7 +7030,7 @@
     </row>
     <row r="38" outlineLevel="2">
       <c r="A38" s="284" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="B38" s="242">
         <v>5.7602513035</v>
@@ -7018,7 +7086,7 @@
     </row>
     <row r="39" outlineLevel="2">
       <c r="A39" s="284" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="B39" s="242">
         <v>5.75</v>
@@ -7074,7 +7142,7 @@
     </row>
     <row r="40" outlineLevel="2">
       <c r="A40" s="289" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="B40" s="242">
         <v>7.6157673173</v>
@@ -7130,7 +7198,7 @@
     </row>
     <row r="41" outlineLevel="2">
       <c r="A41" s="289" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="B41" s="242">
         <v>7.6157673173000004</v>
@@ -7186,7 +7254,7 @@
     </row>
     <row r="42" outlineLevel="2">
       <c r="A42" s="290" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="B42" s="286">
         <v>7.6157673173</v>
@@ -7242,7 +7310,7 @@
     </row>
     <row r="43" outlineLevel="2">
       <c r="A43" s="284" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="B43" s="242">
         <v>5.9518943296</v>
@@ -7298,7 +7366,7 @@
     </row>
     <row r="44" outlineLevel="1">
       <c r="A44" s="285" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="B44" s="286">
         <v>5.9186654191109449</v>
@@ -7354,13 +7422,13 @@
     </row>
     <row r="45" outlineLevel="2">
       <c r="A45" s="284" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="B45" s="242">
         <v>0</v>
       </c>
       <c r="C45" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D45" s="241">
         <v>1618</v>
@@ -7410,13 +7478,13 @@
     </row>
     <row r="46" outlineLevel="2">
       <c r="A46" s="284" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="B46" s="242">
         <v>0</v>
       </c>
       <c r="C46" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D46" s="241">
         <v>81</v>
@@ -7466,13 +7534,13 @@
     </row>
     <row r="47" outlineLevel="2">
       <c r="A47" s="284" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="B47" s="242">
         <v>0</v>
       </c>
       <c r="C47" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D47" s="241">
         <v>1209</v>
@@ -7522,13 +7590,13 @@
     </row>
     <row r="48" outlineLevel="2">
       <c r="A48" s="284" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="B48" s="242">
         <v>0</v>
       </c>
       <c r="C48" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D48" s="241">
         <v>-725</v>
@@ -7578,13 +7646,13 @@
     </row>
     <row r="49" outlineLevel="1">
       <c r="A49" s="285" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="B49" s="286">
         <v>0</v>
       </c>
       <c r="C49" s="295" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D49" s="287">
         <v>2183</v>
@@ -7634,7 +7702,7 @@
     </row>
     <row r="50">
       <c r="A50" s="296" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="B50" s="286">
         <v>5.170114552357802</v>
@@ -7690,7 +7758,7 @@
     </row>
     <row r="52">
       <c r="A52" s="269" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="B52" s="270"/>
       <c r="C52" s="270"/>
@@ -7712,7 +7780,7 @@
     </row>
     <row r="53" outlineLevel="2">
       <c r="A53" s="284" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="B53" s="242">
         <v>1.19556979049893</v>
@@ -7768,13 +7836,13 @@
     </row>
     <row r="54" outlineLevel="2">
       <c r="A54" s="284" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="B54" s="242">
         <v>0.80152102589999985</v>
       </c>
       <c r="C54" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D54" s="241">
         <v>1726.2027071345299</v>
@@ -7824,13 +7892,13 @@
     </row>
     <row r="55" outlineLevel="2">
       <c r="A55" s="284" t="s">
-        <v>89</v>
+        <v>147</v>
       </c>
       <c r="B55" s="242">
         <v>0.8015210259</v>
       </c>
       <c r="C55" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D55" s="241">
         <v>25001.620562999502</v>
@@ -7880,13 +7948,13 @@
     </row>
     <row r="56" outlineLevel="2">
       <c r="A56" s="284" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
       <c r="B56" s="242">
         <v>0.281119982</v>
       </c>
       <c r="C56" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D56" s="241">
         <v>8980.37824203244</v>
@@ -7936,13 +8004,13 @@
     </row>
     <row r="57" outlineLevel="2">
       <c r="A57" s="284" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
       <c r="B57" s="242">
         <v>0</v>
       </c>
       <c r="C57" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D57" s="241">
         <v>15449.5638268403</v>
@@ -7992,7 +8060,7 @@
     </row>
     <row r="58" outlineLevel="1">
       <c r="A58" s="285" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="B58" s="286">
         <v>0.79455040871786742</v>
@@ -8048,13 +8116,13 @@
     </row>
     <row r="59" outlineLevel="2">
       <c r="A59" s="284" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="B59" s="242">
         <v>0</v>
       </c>
       <c r="C59" s="272" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D59" s="241">
         <v>371</v>
@@ -8104,13 +8172,13 @@
     </row>
     <row r="60" outlineLevel="1">
       <c r="A60" s="285" t="s">
-        <v>93</v>
+        <v>151</v>
       </c>
       <c r="B60" s="286">
         <v>0</v>
       </c>
       <c r="C60" s="295" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="D60" s="287">
         <v>371</v>
@@ -8160,7 +8228,7 @@
     </row>
     <row r="61">
       <c r="A61" s="296" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="B61" s="286">
         <v>0.79135050639771976</v>
@@ -8216,7 +8284,7 @@
     </row>
     <row r="63">
       <c r="A63" s="269" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="B63" s="270"/>
       <c r="C63" s="270"/>
@@ -8238,7 +8306,7 @@
     </row>
     <row r="64">
       <c r="A64" s="296" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="B64" s="286">
         <v>37.543800160535064</v>
@@ -8338,7 +8406,7 @@
   <sheetData>
     <row r="1" ht="24.95" customHeight="1" s="230" customFormat="1">
       <c r="A1" s="262" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="B1" s="262"/>
       <c r="C1" s="262"/>
@@ -8362,58 +8430,58 @@
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="244" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="227" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="227" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="227" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="227" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="227" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="227" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="227" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="227" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="227" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="244"/>
       <c r="E14" s="227" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="G14" s="227" t="s">
         <v>24</v>
@@ -8492,7 +8560,7 @@
     </row>
     <row r="26" ht="72.75" customHeight="1">
       <c r="A26" s="261" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="B26" s="261"/>
       <c r="C26" s="261"/>
@@ -8516,48 +8584,48 @@
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="A28" s="227" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1">
       <c r="B29" s="245" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="C29" s="245" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="D29" s="245" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="E29" s="245" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="F29" s="245" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="G29" s="245" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="H29" s="245" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="I29" s="245" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="J29" s="245" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="K29" s="245" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="L29" s="245" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="M29" s="245" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="N29" s="245" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1">
@@ -8603,7 +8671,7 @@
     </row>
     <row r="31" ht="15" customHeight="1">
       <c r="B31" s="245" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="C31" s="245">
         <v>300</v>
@@ -8644,7 +8712,7 @@
     </row>
     <row r="33" ht="30" customHeight="1">
       <c r="A33" s="261" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="B33" s="261"/>
       <c r="C33" s="261"/>
@@ -8666,15 +8734,15 @@
     </row>
     <row r="35" ht="15" customHeight="1">
       <c r="A35" s="227" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1">
       <c r="E37" s="227" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="F37" s="227" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1">
@@ -8833,7 +8901,7 @@
     </row>
     <row r="53" ht="57.75" customHeight="1">
       <c r="A53" s="261" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="B53" s="261"/>
       <c r="C53" s="261"/>
@@ -8854,7 +8922,7 @@
     </row>
     <row r="54" ht="44.25" customHeight="1">
       <c r="A54" s="261" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="B54" s="261"/>
       <c r="C54" s="261"/>
@@ -8894,112 +8962,112 @@
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" s="244" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="227" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="227" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="227" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="227" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="227" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="227" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="227" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="227" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="227" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="227" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="227" t="s">
-        <v>139</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="227" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="227" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="227" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="227" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="227" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="227" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="227" t="s">
-        <v>146</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="227" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="227" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="227" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -9055,7 +9123,7 @@
   <sheetData>
     <row r="1" ht="24.75">
       <c r="A1" s="263" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="B1" s="263"/>
       <c r="C1" s="263"/>

</xml_diff>